<commit_message>
Refactoring and status panel
</commit_message>
<xml_diff>
--- a/doc/temporal.xlsx
+++ b/doc/temporal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CCONTA\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD45D9CE-F25C-4757-97E6-2E83D17D201D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B314FFF9-8F03-49BF-8005-9FF2DC33938B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{8DAE0E3B-ADD7-41D6-ADA2-4B26E4D51ADD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Hogar</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>Tubos</t>
+  </si>
+  <si>
+    <t>Paquete</t>
+  </si>
+  <si>
+    <t>Cervezas con Juanma</t>
+  </si>
+  <si>
+    <t>Tabaco de liar</t>
+  </si>
+  <si>
+    <t>Ecofamily</t>
+  </si>
+  <si>
+    <t>Comida hostal</t>
+  </si>
+  <si>
+    <t>Kebak</t>
+  </si>
+  <si>
+    <t>Comida</t>
   </si>
 </sst>
 </file>
@@ -613,10 +634,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDD5D64-ED3E-4A80-ADF8-1465D0184664}">
-  <dimension ref="A2:D7"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,6 +723,146 @@
         <v>23</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44818</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44818</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44818</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44819</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>44820</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44819</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44821</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44820</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>44820</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>44820</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>